<commit_message>
Excel Report API - add write tasks methods and others to the Excel_Repot CLASS
</commit_message>
<xml_diff>
--- a/media/Reports/Tomer.xlsx
+++ b/media/Reports/Tomer.xlsx
@@ -13,10 +13,149 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="42">
+  <si>
+    <t>Problem</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Date_Created</t>
+  </si>
+  <si>
+    <t>Start Date</t>
+  </si>
+  <si>
+    <t>Email attached file</t>
+  </si>
+  <si>
+    <t>ללכת לאכול בפארק</t>
+  </si>
+  <si>
+    <t>רעב רצחחחחחחחח חיייייייבבבב אוכלללללל</t>
+  </si>
+  <si>
+    <t>2021-01-20 20:35:26.623884+00:00</t>
+  </si>
+  <si>
+    <t>2021-01-21 22:35:00+00:00</t>
+  </si>
+  <si>
+    <t>Emails_Files_Tasks/Ht.png</t>
+  </si>
+  <si>
+    <t>סו ושמחו , בשמחת תורה</t>
+  </si>
+  <si>
+    <t>הייייייי אי ניייד סומבאדייי היייי</t>
+  </si>
+  <si>
+    <t>2021-01-20 20:46:39.909970+00:00</t>
+  </si>
+  <si>
+    <t>2021-01-20 22:46:00+00:00</t>
+  </si>
+  <si>
+    <t>Emails_Files_Tasks/Ht_XpPHx39.png</t>
+  </si>
+  <si>
+    <t>Tomer Test</t>
+  </si>
+  <si>
+    <t>גדשגדשגדשגדשגדגדשגדש</t>
+  </si>
+  <si>
+    <t>2021-01-20 20:47:15.406410+00:00</t>
+  </si>
+  <si>
+    <t>2021-01-09 22:47:00+00:00</t>
+  </si>
+  <si>
+    <t>Emails_Files_Tasks/ClearBitAPI_VwWZRui.PNG</t>
+  </si>
+  <si>
+    <t>Hello World</t>
+  </si>
+  <si>
+    <t>hello hello hellp</t>
+  </si>
+  <si>
+    <t>2021-01-26 18:34:36.136413+00:00</t>
+  </si>
+  <si>
+    <t>2021-02-02 20:33:00+00:00</t>
+  </si>
+  <si>
+    <t>Emails_Files_Tasks/ClearBitAPI_W55aLN4.PNG</t>
+  </si>
+  <si>
+    <t>DUDU topaz</t>
+  </si>
+  <si>
+    <t>wassuppppp</t>
+  </si>
+  <si>
+    <t>2021-01-27 23:16:57.643539+00:00</t>
+  </si>
+  <si>
+    <t>2021-01-01 01:16:00+00:00</t>
+  </si>
+  <si>
+    <t>No File Attached</t>
+  </si>
+  <si>
+    <t>eat alot of food</t>
+  </si>
+  <si>
+    <t>PIZZAA PIZAAA PIZZZA</t>
+  </si>
+  <si>
+    <t>2021-01-27 23:21:29.633551+00:00</t>
+  </si>
+  <si>
+    <t>2021-01-02 01:21:00+00:00</t>
+  </si>
+  <si>
+    <t>Eat Eat</t>
+  </si>
+  <si>
+    <t>Eattttttttttttttttttt</t>
+  </si>
+  <si>
+    <t>2021-01-28 13:41:34.927048+00:00</t>
+  </si>
+  <si>
+    <t>2021-01-04 15:41:00+00:00</t>
+  </si>
+  <si>
+    <t>לאכולללללללללללללללללללל</t>
+  </si>
+  <si>
+    <t>לאכול לאכול מלא אוכל לאכול</t>
+  </si>
+  <si>
+    <t>2021-01-28 13:46:37.974221+00:00</t>
+  </si>
+  <si>
+    <t>2021-01-11 15:44:00+00:00</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <fonts count="2">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -44,8 +183,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -340,12 +480,166 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" t="s">
+        <v>27</v>
+      </c>
+      <c r="D6" t="s">
+        <v>28</v>
+      </c>
+      <c r="E6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C7" t="s">
+        <v>32</v>
+      </c>
+      <c r="D7" t="s">
+        <v>33</v>
+      </c>
+      <c r="E7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C8" t="s">
+        <v>36</v>
+      </c>
+      <c r="D8" t="s">
+        <v>37</v>
+      </c>
+      <c r="E8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" t="s">
+        <v>38</v>
+      </c>
+      <c r="B9" t="s">
+        <v>39</v>
+      </c>
+      <c r="C9" t="s">
+        <v>40</v>
+      </c>
+      <c r="D9" t="s">
+        <v>41</v>
+      </c>
+      <c r="E9" t="s">
+        <v>29</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Start styling the Excel_Report headers
</commit_message>
<xml_diff>
--- a/media/Reports/Tomer.xlsx
+++ b/media/Reports/Tomer.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="81">
   <si>
     <t>Problem</t>
   </si>
@@ -46,6 +46,84 @@
     <t>Emails_Files_Tasks/Ht.png</t>
   </si>
   <si>
+    <t>Mission</t>
+  </si>
+  <si>
+    <t>Responsibility</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>status</t>
+  </si>
+  <si>
+    <t>fdsfdsfds</t>
+  </si>
+  <si>
+    <t>דגדשגדשגדש</t>
+  </si>
+  <si>
+    <t>גדשגדש</t>
+  </si>
+  <si>
+    <t>benharushtomer@gmail.com</t>
+  </si>
+  <si>
+    <t>Open</t>
+  </si>
+  <si>
+    <t>גדשגדשגדשגדשבסזבסז</t>
+  </si>
+  <si>
+    <t>דגדשגדשגדשבסזבסז</t>
+  </si>
+  <si>
+    <t>גדשגדשגדשגדש</t>
+  </si>
+  <si>
+    <t>Closed</t>
+  </si>
+  <si>
+    <t>fdsfds</t>
+  </si>
+  <si>
+    <t>cxzcxz</t>
+  </si>
+  <si>
+    <t>cxzcxzcxz</t>
+  </si>
+  <si>
+    <t>dsadsadsadsadsa</t>
+  </si>
+  <si>
+    <t>dsadsadsadsadsadsa</t>
+  </si>
+  <si>
+    <t>dsadsadsa</t>
+  </si>
+  <si>
+    <t>dudu@gmail.com</t>
+  </si>
+  <si>
+    <t>fdsfdsfdsfs</t>
+  </si>
+  <si>
+    <t>fsdfdsfds</t>
+  </si>
+  <si>
+    <t>Audi@gfgfdgfd.com</t>
+  </si>
+  <si>
+    <t>dasdasdsa</t>
+  </si>
+  <si>
+    <t>dsadsa</t>
+  </si>
+  <si>
+    <t>Stuck</t>
+  </si>
+  <si>
     <t>סו ושמחו , בשמחת תורה</t>
   </si>
   <si>
@@ -91,6 +169,9 @@
     <t>Emails_Files_Tasks/ClearBitAPI_W55aLN4.PNG</t>
   </si>
   <si>
+    <t>fdsdsfds</t>
+  </si>
+  <si>
     <t>DUDU topaz</t>
   </si>
   <si>
@@ -106,6 +187,24 @@
     <t>No File Attached</t>
   </si>
   <si>
+    <t>adsadsadsa</t>
+  </si>
+  <si>
+    <t>dsadsad</t>
+  </si>
+  <si>
+    <t>Saab@gfgfd.com</t>
+  </si>
+  <si>
+    <t>dsadsadsadsxz</t>
+  </si>
+  <si>
+    <t>adsadsadsadsadsa</t>
+  </si>
+  <si>
+    <t>dsadsaddsadsa</t>
+  </si>
+  <si>
     <t>eat alot of food</t>
   </si>
   <si>
@@ -118,6 +217,21 @@
     <t>2021-01-02 01:21:00+00:00</t>
   </si>
   <si>
+    <t>DSADSADSA</t>
+  </si>
+  <si>
+    <t>dsadas@gmail.com</t>
+  </si>
+  <si>
+    <t>fuel</t>
+  </si>
+  <si>
+    <t>go with the car</t>
+  </si>
+  <si>
+    <t>dor</t>
+  </si>
+  <si>
     <t>Eat Eat</t>
   </si>
   <si>
@@ -128,6 +242,9 @@
   </si>
   <si>
     <t>2021-01-04 15:41:00+00:00</t>
+  </si>
+  <si>
+    <t>dasdsadsa</t>
   </si>
   <si>
     <t>לאכולללללללללללללללללללל</t>
@@ -163,12 +280,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCAE3FB"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -185,7 +308,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -480,13 +603,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:J37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:10">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -503,7 +626,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:10">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -520,123 +643,599 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
-      <c r="A3" t="s">
+    <row r="3" spans="1:10">
+      <c r="F3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B3" t="s">
+      <c r="H3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C3" t="s">
+      <c r="I3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D3" t="s">
+      <c r="J3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E3" t="s">
+    </row>
+    <row r="4" spans="1:10">
+      <c r="F4" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" t="s">
+      <c r="G4" t="s">
         <v>15</v>
       </c>
-      <c r="B4" t="s">
+      <c r="H4" t="s">
         <v>16</v>
       </c>
-      <c r="C4" t="s">
+      <c r="I4" t="s">
         <v>17</v>
       </c>
-      <c r="D4" t="s">
+      <c r="J4" t="s">
         <v>18</v>
       </c>
-      <c r="E4" t="s">
+    </row>
+    <row r="5" spans="1:10">
+      <c r="F5" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" t="s">
+      <c r="G5" t="s">
         <v>20</v>
       </c>
-      <c r="B5" t="s">
+      <c r="H5" t="s">
         <v>21</v>
       </c>
-      <c r="C5" t="s">
+      <c r="I5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J5" t="s">
         <v>22</v>
       </c>
-      <c r="D5" t="s">
+    </row>
+    <row r="6" spans="1:10">
+      <c r="F6" t="s">
+        <v>19</v>
+      </c>
+      <c r="G6" t="s">
+        <v>20</v>
+      </c>
+      <c r="H6" t="s">
+        <v>21</v>
+      </c>
+      <c r="I6" t="s">
+        <v>17</v>
+      </c>
+      <c r="J6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="F7" t="s">
         <v>23</v>
       </c>
-      <c r="E5" t="s">
+      <c r="G7" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6" t="s">
+      <c r="H7" t="s">
         <v>25</v>
       </c>
-      <c r="B6" t="s">
+      <c r="I7" t="s">
+        <v>17</v>
+      </c>
+      <c r="J7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="F8" t="s">
         <v>26</v>
       </c>
-      <c r="C6" t="s">
+      <c r="G8" t="s">
         <v>27</v>
       </c>
-      <c r="D6" t="s">
+      <c r="H8" t="s">
         <v>28</v>
       </c>
-      <c r="E6" t="s">
+      <c r="I8" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7" t="s">
+      <c r="J8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
+      <c r="F9" t="s">
         <v>30</v>
       </c>
-      <c r="B7" t="s">
+      <c r="G9" t="s">
+        <v>14</v>
+      </c>
+      <c r="H9" t="s">
         <v>31</v>
       </c>
-      <c r="C7" t="s">
+      <c r="I9" t="s">
         <v>32</v>
       </c>
-      <c r="D7" t="s">
+      <c r="J9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
+      <c r="F10" t="s">
         <v>33</v>
       </c>
-      <c r="E7" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="A8" t="s">
+      <c r="G10" t="s">
+        <v>28</v>
+      </c>
+      <c r="H10" t="s">
         <v>34</v>
       </c>
-      <c r="B8" t="s">
+      <c r="I10" t="s">
+        <v>17</v>
+      </c>
+      <c r="J10" t="s">
         <v>35</v>
       </c>
-      <c r="C8" t="s">
+    </row>
+    <row r="11" spans="1:10">
+      <c r="A11" t="s">
         <v>36</v>
       </c>
-      <c r="D8" t="s">
+      <c r="B11" t="s">
         <v>37</v>
       </c>
-      <c r="E8" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="A9" t="s">
+      <c r="C11" t="s">
         <v>38</v>
       </c>
-      <c r="B9" t="s">
+      <c r="D11" t="s">
         <v>39</v>
       </c>
-      <c r="C9" t="s">
+      <c r="E11" t="s">
         <v>40</v>
       </c>
-      <c r="D9" t="s">
+    </row>
+    <row r="12" spans="1:10">
+      <c r="A12" t="s">
         <v>41</v>
       </c>
-      <c r="E9" t="s">
-        <v>29</v>
+      <c r="B12" t="s">
+        <v>42</v>
+      </c>
+      <c r="C12" t="s">
+        <v>43</v>
+      </c>
+      <c r="D12" t="s">
+        <v>44</v>
+      </c>
+      <c r="E12" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
+      <c r="A13" t="s">
+        <v>46</v>
+      </c>
+      <c r="B13" t="s">
+        <v>47</v>
+      </c>
+      <c r="C13" t="s">
+        <v>48</v>
+      </c>
+      <c r="D13" t="s">
+        <v>49</v>
+      </c>
+      <c r="E13" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10">
+      <c r="F14" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10">
+      <c r="F15" t="s">
+        <v>14</v>
+      </c>
+      <c r="G15" t="s">
+        <v>14</v>
+      </c>
+      <c r="H15" t="s">
+        <v>51</v>
+      </c>
+      <c r="I15" t="s">
+        <v>17</v>
+      </c>
+      <c r="J15" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10">
+      <c r="A16" t="s">
+        <v>52</v>
+      </c>
+      <c r="B16" t="s">
+        <v>53</v>
+      </c>
+      <c r="C16" t="s">
+        <v>54</v>
+      </c>
+      <c r="D16" t="s">
+        <v>55</v>
+      </c>
+      <c r="E16" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10">
+      <c r="F17" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J17" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10">
+      <c r="F18" t="s">
+        <v>28</v>
+      </c>
+      <c r="G18" t="s">
+        <v>57</v>
+      </c>
+      <c r="H18" t="s">
+        <v>58</v>
+      </c>
+      <c r="I18" t="s">
+        <v>59</v>
+      </c>
+      <c r="J18" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10">
+      <c r="F19" t="s">
+        <v>60</v>
+      </c>
+      <c r="G19" t="s">
+        <v>61</v>
+      </c>
+      <c r="H19" t="s">
+        <v>62</v>
+      </c>
+      <c r="I19" t="s">
+        <v>59</v>
+      </c>
+      <c r="J19" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10">
+      <c r="F20" t="s">
+        <v>60</v>
+      </c>
+      <c r="G20" t="s">
+        <v>61</v>
+      </c>
+      <c r="H20" t="s">
+        <v>62</v>
+      </c>
+      <c r="I20" t="s">
+        <v>59</v>
+      </c>
+      <c r="J20" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10">
+      <c r="A21" t="s">
+        <v>63</v>
+      </c>
+      <c r="B21" t="s">
+        <v>64</v>
+      </c>
+      <c r="C21" t="s">
+        <v>65</v>
+      </c>
+      <c r="D21" t="s">
+        <v>66</v>
+      </c>
+      <c r="E21" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10">
+      <c r="F22" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I22" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J22" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10">
+      <c r="F23" t="s">
+        <v>67</v>
+      </c>
+      <c r="G23" t="s">
+        <v>67</v>
+      </c>
+      <c r="H23" t="s">
+        <v>67</v>
+      </c>
+      <c r="I23" t="s">
+        <v>68</v>
+      </c>
+      <c r="J23" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10">
+      <c r="F24" t="s">
+        <v>69</v>
+      </c>
+      <c r="G24" t="s">
+        <v>70</v>
+      </c>
+      <c r="H24" t="s">
+        <v>71</v>
+      </c>
+      <c r="I24" t="s">
+        <v>68</v>
+      </c>
+      <c r="J24" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10">
+      <c r="F25" t="s">
+        <v>69</v>
+      </c>
+      <c r="G25" t="s">
+        <v>70</v>
+      </c>
+      <c r="H25" t="s">
+        <v>71</v>
+      </c>
+      <c r="I25" t="s">
+        <v>68</v>
+      </c>
+      <c r="J25" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10">
+      <c r="F26" t="s">
+        <v>69</v>
+      </c>
+      <c r="G26" t="s">
+        <v>70</v>
+      </c>
+      <c r="H26" t="s">
+        <v>71</v>
+      </c>
+      <c r="I26" t="s">
+        <v>68</v>
+      </c>
+      <c r="J26" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10">
+      <c r="A27" t="s">
+        <v>72</v>
+      </c>
+      <c r="B27" t="s">
+        <v>73</v>
+      </c>
+      <c r="C27" t="s">
+        <v>74</v>
+      </c>
+      <c r="D27" t="s">
+        <v>75</v>
+      </c>
+      <c r="E27" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10">
+      <c r="F28" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I28" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J28" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10">
+      <c r="F29" t="s">
+        <v>28</v>
+      </c>
+      <c r="G29" t="s">
+        <v>28</v>
+      </c>
+      <c r="H29" t="s">
+        <v>76</v>
+      </c>
+      <c r="I29" t="s">
+        <v>17</v>
+      </c>
+      <c r="J29" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10">
+      <c r="F30" t="s">
+        <v>28</v>
+      </c>
+      <c r="G30" t="s">
+        <v>28</v>
+      </c>
+      <c r="H30" t="s">
+        <v>76</v>
+      </c>
+      <c r="I30" t="s">
+        <v>17</v>
+      </c>
+      <c r="J30" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10">
+      <c r="F31" t="s">
+        <v>28</v>
+      </c>
+      <c r="G31" t="s">
+        <v>28</v>
+      </c>
+      <c r="H31" t="s">
+        <v>76</v>
+      </c>
+      <c r="I31" t="s">
+        <v>17</v>
+      </c>
+      <c r="J31" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10">
+      <c r="A32" t="s">
+        <v>77</v>
+      </c>
+      <c r="B32" t="s">
+        <v>78</v>
+      </c>
+      <c r="C32" t="s">
+        <v>79</v>
+      </c>
+      <c r="D32" t="s">
+        <v>80</v>
+      </c>
+      <c r="E32" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="33" spans="6:10">
+      <c r="F33" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H33" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I33" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J33" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="34" spans="6:10">
+      <c r="F34" t="s">
+        <v>14</v>
+      </c>
+      <c r="G34" t="s">
+        <v>14</v>
+      </c>
+      <c r="H34" t="s">
+        <v>14</v>
+      </c>
+      <c r="I34" t="s">
+        <v>17</v>
+      </c>
+      <c r="J34" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="35" spans="6:10">
+      <c r="F35" t="s">
+        <v>14</v>
+      </c>
+      <c r="G35" t="s">
+        <v>14</v>
+      </c>
+      <c r="H35" t="s">
+        <v>14</v>
+      </c>
+      <c r="I35" t="s">
+        <v>17</v>
+      </c>
+      <c r="J35" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="36" spans="6:10">
+      <c r="F36" t="s">
+        <v>14</v>
+      </c>
+      <c r="G36" t="s">
+        <v>14</v>
+      </c>
+      <c r="H36" t="s">
+        <v>14</v>
+      </c>
+      <c r="I36" t="s">
+        <v>17</v>
+      </c>
+      <c r="J36" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="37" spans="6:10">
+      <c r="F37" t="s">
+        <v>25</v>
+      </c>
+      <c r="G37" t="s">
+        <v>25</v>
+      </c>
+      <c r="H37" t="s">
+        <v>24</v>
+      </c>
+      <c r="I37" t="s">
+        <v>17</v>
+      </c>
+      <c r="J37" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Continue work on the excel Report , add header styling for the task_details headers
</commit_message>
<xml_diff>
--- a/media/Reports/Tomer.xlsx
+++ b/media/Reports/Tomer.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="87">
   <si>
     <t>Problem</t>
   </si>
@@ -247,6 +247,15 @@
     <t>dasdsadsa</t>
   </si>
   <si>
+    <t>bvcbvcbvcbvcbvcsgfgsd</t>
+  </si>
+  <si>
+    <t>cbvcbcvbvc</t>
+  </si>
+  <si>
+    <t>bvcbvcbcv</t>
+  </si>
+  <si>
     <t>לאכולללללללללללללללללללל</t>
   </si>
   <si>
@@ -257,6 +266,15 @@
   </si>
   <si>
     <t>2021-01-11 15:44:00+00:00</t>
+  </si>
+  <si>
+    <t>DUDU</t>
+  </si>
+  <si>
+    <t>vcxvcxvcx</t>
+  </si>
+  <si>
+    <t>vcxvcx@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -280,7 +298,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -290,6 +308,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFCAE3FB"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF8080"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -306,9 +330,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -603,7 +628,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J37"/>
+  <dimension ref="A1:J40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -644,19 +669,19 @@
       </c>
     </row>
     <row r="3" spans="1:10">
-      <c r="F3" s="1" t="s">
+      <c r="F3" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="G3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="H3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="I3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="J3" s="1" t="s">
+      <c r="J3" s="2" t="s">
         <v>13</v>
       </c>
     </row>
@@ -831,19 +856,19 @@
       </c>
     </row>
     <row r="14" spans="1:10">
-      <c r="F14" s="1" t="s">
+      <c r="F14" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="G14" s="1" t="s">
+      <c r="G14" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="H14" s="1" t="s">
+      <c r="H14" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I14" s="1" t="s">
+      <c r="I14" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="J14" s="1" t="s">
+      <c r="J14" s="2" t="s">
         <v>13</v>
       </c>
     </row>
@@ -882,19 +907,19 @@
       </c>
     </row>
     <row r="17" spans="1:10">
-      <c r="F17" s="1" t="s">
+      <c r="F17" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="G17" s="1" t="s">
+      <c r="G17" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="H17" s="1" t="s">
+      <c r="H17" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I17" s="1" t="s">
+      <c r="I17" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="J17" s="1" t="s">
+      <c r="J17" s="2" t="s">
         <v>13</v>
       </c>
     </row>
@@ -967,19 +992,19 @@
       </c>
     </row>
     <row r="22" spans="1:10">
-      <c r="F22" s="1" t="s">
+      <c r="F22" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="G22" s="1" t="s">
+      <c r="G22" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="H22" s="1" t="s">
+      <c r="H22" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I22" s="1" t="s">
+      <c r="I22" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="J22" s="1" t="s">
+      <c r="J22" s="2" t="s">
         <v>13</v>
       </c>
     </row>
@@ -1069,19 +1094,19 @@
       </c>
     </row>
     <row r="28" spans="1:10">
-      <c r="F28" s="1" t="s">
+      <c r="F28" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="G28" s="1" t="s">
+      <c r="G28" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="H28" s="1" t="s">
+      <c r="H28" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I28" s="1" t="s">
+      <c r="I28" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="J28" s="1" t="s">
+      <c r="J28" s="2" t="s">
         <v>13</v>
       </c>
     </row>
@@ -1137,57 +1162,57 @@
       </c>
     </row>
     <row r="32" spans="1:10">
-      <c r="A32" t="s">
+      <c r="F32" t="s">
         <v>77</v>
       </c>
-      <c r="B32" t="s">
+      <c r="G32" t="s">
         <v>78</v>
       </c>
-      <c r="C32" t="s">
+      <c r="H32" t="s">
         <v>79</v>
       </c>
-      <c r="D32" t="s">
+      <c r="I32" t="s">
+        <v>59</v>
+      </c>
+      <c r="J32" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10">
+      <c r="A33" t="s">
         <v>80</v>
       </c>
-      <c r="E32" t="s">
+      <c r="B33" t="s">
+        <v>81</v>
+      </c>
+      <c r="C33" t="s">
+        <v>82</v>
+      </c>
+      <c r="D33" t="s">
+        <v>83</v>
+      </c>
+      <c r="E33" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="33" spans="6:10">
-      <c r="F33" s="1" t="s">
+    <row r="34" spans="1:10">
+      <c r="F34" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="G33" s="1" t="s">
+      <c r="G34" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="H33" s="1" t="s">
+      <c r="H34" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I33" s="1" t="s">
+      <c r="I34" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="J33" s="1" t="s">
+      <c r="J34" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="34" spans="6:10">
-      <c r="F34" t="s">
-        <v>14</v>
-      </c>
-      <c r="G34" t="s">
-        <v>14</v>
-      </c>
-      <c r="H34" t="s">
-        <v>14</v>
-      </c>
-      <c r="I34" t="s">
-        <v>17</v>
-      </c>
-      <c r="J34" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="35" spans="6:10">
+    <row r="35" spans="1:10">
       <c r="F35" t="s">
         <v>14</v>
       </c>
@@ -1204,7 +1229,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="36" spans="6:10">
+    <row r="36" spans="1:10">
       <c r="F36" t="s">
         <v>14</v>
       </c>
@@ -1218,23 +1243,71 @@
         <v>17</v>
       </c>
       <c r="J36" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="37" spans="6:10">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10">
       <c r="F37" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="G37" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="H37" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="I37" t="s">
         <v>17</v>
       </c>
       <c r="J37" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10">
+      <c r="F38" t="s">
+        <v>25</v>
+      </c>
+      <c r="G38" t="s">
+        <v>25</v>
+      </c>
+      <c r="H38" t="s">
+        <v>24</v>
+      </c>
+      <c r="I38" t="s">
+        <v>17</v>
+      </c>
+      <c r="J38" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10">
+      <c r="F39" t="s">
+        <v>25</v>
+      </c>
+      <c r="G39" t="s">
+        <v>25</v>
+      </c>
+      <c r="H39" t="s">
+        <v>84</v>
+      </c>
+      <c r="I39" t="s">
+        <v>17</v>
+      </c>
+      <c r="J39" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10">
+      <c r="F40" t="s">
+        <v>85</v>
+      </c>
+      <c r="G40" t="s">
+        <v>85</v>
+      </c>
+      <c r="I40" t="s">
+        <v>86</v>
+      </c>
+      <c r="J40" t="s">
         <v>22</v>
       </c>
     </row>

</xml_diff>

<commit_message>
finished to create the xlsx algoritm, and create ReportObject(table)
</commit_message>
<xml_diff>
--- a/media/Reports/Tomer.xlsx
+++ b/media/Reports/Tomer.xlsx
@@ -8,13 +8,14 @@
   </bookViews>
   <sheets>
     <sheet name="Reports" sheetId="1" r:id="rId1"/>
+    <sheet name="Analytical" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="89">
   <si>
     <t>Problem</t>
   </si>
@@ -124,6 +125,9 @@
     <t>Stuck</t>
   </si>
   <si>
+    <t>Task Problem</t>
+  </si>
+  <si>
     <t>סו ושמחו , בשמחת תורה</t>
   </si>
   <si>
@@ -275,6 +279,9 @@
   </si>
   <si>
     <t>vcxvcx@gmail.com</t>
+  </si>
+  <si>
+    <t>vcxvcx</t>
   </si>
 </sst>
 </file>
@@ -341,6 +348,1203 @@
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Problem - ללכת לאכול בפארק</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>tasks status pie</c:v>
+          </c:tx>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FF4500"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FFFF00"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="00FF00"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:dPt>
+          <c:cat>
+            <c:strRef>
+              <c:f>Analytical!$B$1:$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Open</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Stuck</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Closed</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Analytical!$B$2:$D$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr rtl="0">
+            <a:defRPr/>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Problem - סו ושמחו , בשמחת תורה</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>tasks status pie</c:v>
+          </c:tx>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FF4500"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FFFF00"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="00FF00"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:dPt>
+          <c:cat>
+            <c:strRef>
+              <c:f>Analytical!$B$17:$D$17</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Open</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Stuck</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Closed</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Analytical!$B$18:$D$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr rtl="0">
+            <a:defRPr/>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Problem - Tomer Test</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>tasks status pie</c:v>
+          </c:tx>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FF4500"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FFFF00"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="00FF00"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:dPt>
+          <c:cat>
+            <c:strRef>
+              <c:f>Analytical!$B$33:$D$33</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Open</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Stuck</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Closed</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Analytical!$B$34:$D$34</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr rtl="0">
+            <a:defRPr/>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Problem - Hello World</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>tasks status pie</c:v>
+          </c:tx>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FF4500"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FFFF00"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="00FF00"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:dPt>
+          <c:cat>
+            <c:strRef>
+              <c:f>Analytical!$B$49:$D$49</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Open</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Stuck</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Closed</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Analytical!$B$50:$D$50</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr rtl="0">
+            <a:defRPr/>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Problem - DUDU topaz</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>tasks status pie</c:v>
+          </c:tx>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FF4500"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FFFF00"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="00FF00"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:dPt>
+          <c:cat>
+            <c:strRef>
+              <c:f>Analytical!$B$65:$D$65</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Open</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Stuck</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Closed</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Analytical!$B$66:$D$66</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr rtl="0">
+            <a:defRPr/>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Problem - eat alot of food</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>tasks status pie</c:v>
+          </c:tx>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FF4500"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FFFF00"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="00FF00"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:dPt>
+          <c:cat>
+            <c:strRef>
+              <c:f>Analytical!$B$81:$D$81</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Open</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Stuck</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Closed</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Analytical!$B$82:$D$82</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr rtl="0">
+            <a:defRPr/>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Problem - Eat Eat</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>tasks status pie</c:v>
+          </c:tx>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FF4500"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FFFF00"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="00FF00"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:dPt>
+          <c:cat>
+            <c:strRef>
+              <c:f>Analytical!$B$97:$D$97</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Open</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Stuck</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Closed</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Analytical!$B$98:$D$98</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr rtl="0">
+            <a:defRPr/>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Problem - לאכולללללללללללללללללללל</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>tasks status pie</c:v>
+          </c:tx>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FF4500"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FFFF00"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="00FF00"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:dPt>
+          <c:cat>
+            <c:strRef>
+              <c:f>Analytical!$B$113:$D$113</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Open</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Stuck</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Closed</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Analytical!$B$114:$D$114</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr rtl="0">
+            <a:defRPr/>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>238125</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>542925</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>238125</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>542925</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>238125</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>542925</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>238125</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>542925</xdr:colOff>
+      <xdr:row>62</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>238125</xdr:colOff>
+      <xdr:row>64</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>542925</xdr:colOff>
+      <xdr:row>78</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Chart 5"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>238125</xdr:colOff>
+      <xdr:row>80</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>542925</xdr:colOff>
+      <xdr:row>94</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="7" name="Chart 6"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>238125</xdr:colOff>
+      <xdr:row>96</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>542925</xdr:colOff>
+      <xdr:row>110</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="8" name="Chart 7"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId7"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>238125</xdr:colOff>
+      <xdr:row>112</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>542925</xdr:colOff>
+      <xdr:row>126</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="9" name="Chart 8"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId8"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -628,7 +1832,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J40"/>
+  <dimension ref="A1:J41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -806,53 +2010,53 @@
     </row>
     <row r="11" spans="1:10">
       <c r="A11" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B11" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C11" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D11" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E11" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="12" spans="1:10">
       <c r="A12" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B12" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C12" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D12" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E12" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="13" spans="1:10">
       <c r="A13" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B13" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C13" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D13" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E13" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="14" spans="1:10">
@@ -880,7 +2084,7 @@
         <v>14</v>
       </c>
       <c r="H15" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="I15" t="s">
         <v>17</v>
@@ -891,19 +2095,19 @@
     </row>
     <row r="16" spans="1:10">
       <c r="A16" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B16" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C16" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D16" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E16" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="17" spans="1:10">
@@ -928,13 +2132,13 @@
         <v>28</v>
       </c>
       <c r="G18" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="H18" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="I18" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="J18" t="s">
         <v>22</v>
@@ -942,16 +2146,16 @@
     </row>
     <row r="19" spans="1:10">
       <c r="F19" t="s">
+        <v>61</v>
+      </c>
+      <c r="G19" t="s">
+        <v>62</v>
+      </c>
+      <c r="H19" t="s">
+        <v>63</v>
+      </c>
+      <c r="I19" t="s">
         <v>60</v>
-      </c>
-      <c r="G19" t="s">
-        <v>61</v>
-      </c>
-      <c r="H19" t="s">
-        <v>62</v>
-      </c>
-      <c r="I19" t="s">
-        <v>59</v>
       </c>
       <c r="J19" t="s">
         <v>22</v>
@@ -959,16 +2163,16 @@
     </row>
     <row r="20" spans="1:10">
       <c r="F20" t="s">
+        <v>61</v>
+      </c>
+      <c r="G20" t="s">
+        <v>62</v>
+      </c>
+      <c r="H20" t="s">
+        <v>63</v>
+      </c>
+      <c r="I20" t="s">
         <v>60</v>
-      </c>
-      <c r="G20" t="s">
-        <v>61</v>
-      </c>
-      <c r="H20" t="s">
-        <v>62</v>
-      </c>
-      <c r="I20" t="s">
-        <v>59</v>
       </c>
       <c r="J20" t="s">
         <v>18</v>
@@ -976,19 +2180,19 @@
     </row>
     <row r="21" spans="1:10">
       <c r="A21" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B21" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C21" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D21" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E21" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="22" spans="1:10">
@@ -1010,16 +2214,16 @@
     </row>
     <row r="23" spans="1:10">
       <c r="F23" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="G23" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="H23" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="I23" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="J23" t="s">
         <v>18</v>
@@ -1027,16 +2231,16 @@
     </row>
     <row r="24" spans="1:10">
       <c r="F24" t="s">
+        <v>70</v>
+      </c>
+      <c r="G24" t="s">
+        <v>71</v>
+      </c>
+      <c r="H24" t="s">
+        <v>72</v>
+      </c>
+      <c r="I24" t="s">
         <v>69</v>
-      </c>
-      <c r="G24" t="s">
-        <v>70</v>
-      </c>
-      <c r="H24" t="s">
-        <v>71</v>
-      </c>
-      <c r="I24" t="s">
-        <v>68</v>
       </c>
       <c r="J24" t="s">
         <v>18</v>
@@ -1044,16 +2248,16 @@
     </row>
     <row r="25" spans="1:10">
       <c r="F25" t="s">
+        <v>70</v>
+      </c>
+      <c r="G25" t="s">
+        <v>71</v>
+      </c>
+      <c r="H25" t="s">
+        <v>72</v>
+      </c>
+      <c r="I25" t="s">
         <v>69</v>
-      </c>
-      <c r="G25" t="s">
-        <v>70</v>
-      </c>
-      <c r="H25" t="s">
-        <v>71</v>
-      </c>
-      <c r="I25" t="s">
-        <v>68</v>
       </c>
       <c r="J25" t="s">
         <v>18</v>
@@ -1061,16 +2265,16 @@
     </row>
     <row r="26" spans="1:10">
       <c r="F26" t="s">
+        <v>70</v>
+      </c>
+      <c r="G26" t="s">
+        <v>71</v>
+      </c>
+      <c r="H26" t="s">
+        <v>72</v>
+      </c>
+      <c r="I26" t="s">
         <v>69</v>
-      </c>
-      <c r="G26" t="s">
-        <v>70</v>
-      </c>
-      <c r="H26" t="s">
-        <v>71</v>
-      </c>
-      <c r="I26" t="s">
-        <v>68</v>
       </c>
       <c r="J26" t="s">
         <v>22</v>
@@ -1078,19 +2282,19 @@
     </row>
     <row r="27" spans="1:10">
       <c r="A27" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B27" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C27" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D27" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="E27" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="28" spans="1:10">
@@ -1118,7 +2322,7 @@
         <v>28</v>
       </c>
       <c r="H29" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="I29" t="s">
         <v>17</v>
@@ -1135,7 +2339,7 @@
         <v>28</v>
       </c>
       <c r="H30" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="I30" t="s">
         <v>17</v>
@@ -1152,7 +2356,7 @@
         <v>28</v>
       </c>
       <c r="H31" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="I31" t="s">
         <v>17</v>
@@ -1163,16 +2367,16 @@
     </row>
     <row r="32" spans="1:10">
       <c r="F32" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="G32" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="H32" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="I32" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="J32" t="s">
         <v>35</v>
@@ -1180,19 +2384,19 @@
     </row>
     <row r="33" spans="1:10">
       <c r="A33" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B33" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C33" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D33" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="E33" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="34" spans="1:10">
@@ -1217,7 +2421,7 @@
         <v>14</v>
       </c>
       <c r="G35" t="s">
-        <v>14</v>
+        <v>34</v>
       </c>
       <c r="H35" t="s">
         <v>14</v>
@@ -1288,7 +2492,7 @@
         <v>25</v>
       </c>
       <c r="H39" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="I39" t="s">
         <v>17</v>
@@ -1299,19 +2503,274 @@
     </row>
     <row r="40" spans="1:10">
       <c r="F40" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="G40" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="I40" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="J40" t="s">
         <v>22</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10">
+      <c r="F41" t="s">
+        <v>88</v>
+      </c>
+      <c r="G41" t="s">
+        <v>88</v>
+      </c>
+      <c r="H41" t="s">
+        <v>88</v>
+      </c>
+      <c r="I41" t="s">
+        <v>17</v>
+      </c>
+      <c r="J41" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D114"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2">
+        <v>3</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B18">
+        <v>0</v>
+      </c>
+      <c r="C18">
+        <v>0</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4">
+      <c r="A33" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4">
+      <c r="A34" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B34">
+        <v>0</v>
+      </c>
+      <c r="C34">
+        <v>0</v>
+      </c>
+      <c r="D34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4">
+      <c r="A49" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4">
+      <c r="A50" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B50">
+        <v>1</v>
+      </c>
+      <c r="C50">
+        <v>0</v>
+      </c>
+      <c r="D50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4">
+      <c r="A65" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D65" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4">
+      <c r="A66" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B66">
+        <v>1</v>
+      </c>
+      <c r="C66">
+        <v>0</v>
+      </c>
+      <c r="D66">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4">
+      <c r="A81" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C81" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D81" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4">
+      <c r="A82" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B82">
+        <v>3</v>
+      </c>
+      <c r="C82">
+        <v>0</v>
+      </c>
+      <c r="D82">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4">
+      <c r="A97" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B97" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C97" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D97" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4">
+      <c r="A98" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B98">
+        <v>2</v>
+      </c>
+      <c r="C98">
+        <v>1</v>
+      </c>
+      <c r="D98">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4">
+      <c r="A113" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B113" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C113" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D113" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4">
+      <c r="A114" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B114">
+        <v>3</v>
+      </c>
+      <c r="C114">
+        <v>1</v>
+      </c>
+      <c r="D114">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
add backend changes in api_xlsx view, now working on the front of the api call for this view
</commit_message>
<xml_diff>
--- a/media/Reports/Tomer.xlsx
+++ b/media/Reports/Tomer.xlsx
@@ -527,7 +527,7 @@
           </c:dPt>
           <c:cat>
             <c:strRef>
-              <c:f>Analytical!$B$17:$D$17</c:f>
+              <c:f>Analytical!$B$16:$D$16</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -544,7 +544,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Analytical!$B$18:$D$18</c:f>
+              <c:f>Analytical!$B$17:$D$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -646,7 +646,7 @@
           </c:dPt>
           <c:cat>
             <c:strRef>
-              <c:f>Analytical!$B$33:$D$33</c:f>
+              <c:f>Analytical!$B$31:$D$31</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -663,7 +663,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Analytical!$B$34:$D$34</c:f>
+              <c:f>Analytical!$B$32:$D$32</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -765,7 +765,7 @@
           </c:dPt>
           <c:cat>
             <c:strRef>
-              <c:f>Analytical!$B$49:$D$49</c:f>
+              <c:f>Analytical!$B$46:$D$46</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -782,7 +782,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Analytical!$B$50:$D$50</c:f>
+              <c:f>Analytical!$B$47:$D$47</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -884,7 +884,7 @@
           </c:dPt>
           <c:cat>
             <c:strRef>
-              <c:f>Analytical!$B$65:$D$65</c:f>
+              <c:f>Analytical!$B$61:$D$61</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -901,7 +901,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Analytical!$B$66:$D$66</c:f>
+              <c:f>Analytical!$B$62:$D$62</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -1003,7 +1003,7 @@
           </c:dPt>
           <c:cat>
             <c:strRef>
-              <c:f>Analytical!$B$81:$D$81</c:f>
+              <c:f>Analytical!$B$76:$D$76</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -1020,7 +1020,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Analytical!$B$82:$D$82</c:f>
+              <c:f>Analytical!$B$77:$D$77</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -1122,7 +1122,7 @@
           </c:dPt>
           <c:cat>
             <c:strRef>
-              <c:f>Analytical!$B$97:$D$97</c:f>
+              <c:f>Analytical!$B$91:$D$91</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -1139,7 +1139,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Analytical!$B$98:$D$98</c:f>
+              <c:f>Analytical!$B$92:$D$92</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -1241,7 +1241,7 @@
           </c:dPt>
           <c:cat>
             <c:strRef>
-              <c:f>Analytical!$B$113:$D$113</c:f>
+              <c:f>Analytical!$B$106:$D$106</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -1258,15 +1258,15 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Analytical!$B$114:$D$114</c:f>
+              <c:f>Analytical!$B$107:$D$107</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>3</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>3</c:v>
@@ -1338,13 +1338,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>238125</xdr:colOff>
-      <xdr:row>16</xdr:row>
+      <xdr:row>15</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
       <xdr:colOff>542925</xdr:colOff>
-      <xdr:row>30</xdr:row>
+      <xdr:row>29</xdr:row>
       <xdr:rowOff>171450</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1368,13 +1368,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>238125</xdr:colOff>
-      <xdr:row>32</xdr:row>
+      <xdr:row>30</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
       <xdr:colOff>542925</xdr:colOff>
-      <xdr:row>46</xdr:row>
+      <xdr:row>44</xdr:row>
       <xdr:rowOff>171450</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1398,13 +1398,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>238125</xdr:colOff>
-      <xdr:row>48</xdr:row>
+      <xdr:row>45</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
       <xdr:colOff>542925</xdr:colOff>
-      <xdr:row>62</xdr:row>
+      <xdr:row>59</xdr:row>
       <xdr:rowOff>171450</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1428,13 +1428,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>238125</xdr:colOff>
-      <xdr:row>64</xdr:row>
+      <xdr:row>60</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
       <xdr:colOff>542925</xdr:colOff>
-      <xdr:row>78</xdr:row>
+      <xdr:row>74</xdr:row>
       <xdr:rowOff>171450</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1458,13 +1458,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>238125</xdr:colOff>
-      <xdr:row>80</xdr:row>
+      <xdr:row>75</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
       <xdr:colOff>542925</xdr:colOff>
-      <xdr:row>94</xdr:row>
+      <xdr:row>89</xdr:row>
       <xdr:rowOff>171450</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1488,13 +1488,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>238125</xdr:colOff>
-      <xdr:row>96</xdr:row>
+      <xdr:row>90</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
       <xdr:colOff>542925</xdr:colOff>
-      <xdr:row>110</xdr:row>
+      <xdr:row>104</xdr:row>
       <xdr:rowOff>171450</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1518,13 +1518,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>238125</xdr:colOff>
-      <xdr:row>112</xdr:row>
+      <xdr:row>105</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
       <xdr:colOff>542925</xdr:colOff>
-      <xdr:row>126</xdr:row>
+      <xdr:row>119</xdr:row>
       <xdr:rowOff>171450</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -2517,7 +2517,7 @@
     </row>
     <row r="41" spans="1:10">
       <c r="F41" t="s">
-        <v>88</v>
+        <v>14</v>
       </c>
       <c r="G41" t="s">
         <v>88</v>
@@ -2529,7 +2529,7 @@
         <v>17</v>
       </c>
       <c r="J41" t="s">
-        <v>18</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -2539,7 +2539,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D114"/>
+  <dimension ref="A1:D107"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2573,199 +2573,199 @@
         <v>3</v>
       </c>
     </row>
+    <row r="16" spans="1:4">
+      <c r="A16" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
     <row r="17" spans="1:4">
       <c r="A17" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B17">
+        <v>0</v>
+      </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4">
+      <c r="A31" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B31" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="C31" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="D31" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
-      <c r="A18" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B18">
+    <row r="32" spans="1:4">
+      <c r="A32" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B32">
         <v>0</v>
       </c>
-      <c r="C18">
+      <c r="C32">
         <v>0</v>
       </c>
-      <c r="D18">
+      <c r="D32">
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:4">
-      <c r="A33" s="1" t="s">
+    <row r="46" spans="1:4">
+      <c r="A46" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B33" s="1" t="s">
+      <c r="B46" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C33" s="1" t="s">
+      <c r="C46" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D33" s="1" t="s">
+      <c r="D46" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="34" spans="1:4">
-      <c r="A34" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B34">
+    <row r="47" spans="1:4">
+      <c r="A47" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B47">
+        <v>1</v>
+      </c>
+      <c r="C47">
         <v>0</v>
       </c>
-      <c r="C34">
+      <c r="D47">
         <v>0</v>
       </c>
-      <c r="D34">
+    </row>
+    <row r="61" spans="1:4">
+      <c r="A61" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4">
+      <c r="A62" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B62">
+        <v>1</v>
+      </c>
+      <c r="C62">
         <v>0</v>
       </c>
-    </row>
-    <row r="49" spans="1:4">
-      <c r="A49" s="1" t="s">
+      <c r="D62">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4">
+      <c r="A76" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B49" s="1" t="s">
+      <c r="B76" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C49" s="1" t="s">
+      <c r="C76" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D49" s="1" t="s">
+      <c r="D76" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="50" spans="1:4">
-      <c r="A50" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="B50">
+    <row r="77" spans="1:4">
+      <c r="A77" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B77">
+        <v>3</v>
+      </c>
+      <c r="C77">
+        <v>0</v>
+      </c>
+      <c r="D77">
         <v>1</v>
       </c>
-      <c r="C50">
-        <v>0</v>
-      </c>
-      <c r="D50">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4">
-      <c r="A65" s="1" t="s">
+    </row>
+    <row r="91" spans="1:4">
+      <c r="A91" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B65" s="1" t="s">
+      <c r="B91" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C65" s="1" t="s">
+      <c r="C91" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D65" s="1" t="s">
+      <c r="D91" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="66" spans="1:4">
-      <c r="A66" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="B66">
+    <row r="92" spans="1:4">
+      <c r="A92" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B92">
+        <v>2</v>
+      </c>
+      <c r="C92">
         <v>1</v>
       </c>
-      <c r="C66">
-        <v>0</v>
-      </c>
-      <c r="D66">
+      <c r="D92">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4">
+      <c r="A106" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B106" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C106" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D106" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4">
+      <c r="A107" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B107">
         <v>2</v>
       </c>
-    </row>
-    <row r="81" spans="1:4">
-      <c r="A81" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B81" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C81" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D81" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="82" spans="1:4">
-      <c r="A82" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="B82">
-        <v>3</v>
-      </c>
-      <c r="C82">
-        <v>0</v>
-      </c>
-      <c r="D82">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="97" spans="1:4">
-      <c r="A97" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B97" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C97" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D97" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="98" spans="1:4">
-      <c r="A98" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="B98">
+      <c r="C107">
         <v>2</v>
       </c>
-      <c r="C98">
-        <v>1</v>
-      </c>
-      <c r="D98">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="113" spans="1:4">
-      <c r="A113" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B113" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C113" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D113" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="114" spans="1:4">
-      <c r="A114" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="B114">
-        <v>3</v>
-      </c>
-      <c r="C114">
-        <v>1</v>
-      </c>
-      <c r="D114">
+      <c r="D107">
         <v>3</v>
       </c>
     </row>

</xml_diff>